<commit_message>
#7 Läuft jetzt ALLES
</commit_message>
<xml_diff>
--- a/Batch_Szenarios.xlsx
+++ b/Batch_Szenarios.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/55b5a83da9441d2b/Business/Ressourcen/GitRepos/M-K/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35E7D29B-4C7C-4EB1-95F5-C9C6FB77E031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{35E7D29B-4C7C-4EB1-95F5-C9C6FB77E031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86C74CF4-1A42-4D7D-9415-6F74CFDB2246}"/>
   <bookViews>
-    <workbookView xWindow="21915" yWindow="2985" windowWidth="27750" windowHeight="13515" xr2:uid="{84012C3F-0F01-4CE2-BC25-ED3D97AAB7AF}"/>
+    <workbookView xWindow="10215" yWindow="4500" windowWidth="37275" windowHeight="13515" xr2:uid="{84012C3F-0F01-4CE2-BC25-ED3D97AAB7AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Batch_Szenarios" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Batch_Szenarios!$A$1:$K$2</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Batch_Szenarios!$A$1:$K$48</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="12">
   <si>
     <t>StartCollateralETH</t>
   </si>
@@ -119,9 +119,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -141,6 +140,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -164,8 +167,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A812C522-97A6-4107-900C-07C7CD2B9918}" name="Batch_Szenarios" displayName="Batch_Szenarios" ref="A1:K2" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:K2" xr:uid="{A812C522-97A6-4107-900C-07C7CD2B9918}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A812C522-97A6-4107-900C-07C7CD2B9918}" name="Batch_Szenarios" displayName="Batch_Szenarios" ref="A1:K48" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:K48" xr:uid="{A812C522-97A6-4107-900C-07C7CD2B9918}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{B4C3076B-C7F1-4587-9C53-10593B212DB0}" uniqueName="1" name="StartCollateralETH" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{8669153E-4C6E-46F4-BF6F-B39D88A4557C}" uniqueName="2" name="ParBänder" queryTableFieldId="2"/>
@@ -480,9 +483,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B72C522-7B1A-48D2-B2EE-FC13DB351A8C}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -553,7 +558,7 @@
       <c r="F2">
         <v>1863.34</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
       <c r="H2">
@@ -566,7 +571,1617 @@
         <v>500</v>
       </c>
       <c r="K2">
-        <v>10000</v>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>1863.34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>1863.34</v>
+      </c>
+      <c r="I3">
+        <v>50</v>
+      </c>
+      <c r="J3">
+        <v>500</v>
+      </c>
+      <c r="K3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>1863.34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4">
+        <v>1863.34</v>
+      </c>
+      <c r="I4">
+        <v>50</v>
+      </c>
+      <c r="J4">
+        <v>500</v>
+      </c>
+      <c r="K4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>1863.34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5">
+        <v>1863.34</v>
+      </c>
+      <c r="I5">
+        <v>50</v>
+      </c>
+      <c r="J5">
+        <v>500</v>
+      </c>
+      <c r="K5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>1863.34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6">
+        <v>1863.34</v>
+      </c>
+      <c r="I6">
+        <v>50</v>
+      </c>
+      <c r="J6">
+        <v>500</v>
+      </c>
+      <c r="K6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>1863.34</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>1863.34</v>
+      </c>
+      <c r="I7">
+        <v>50</v>
+      </c>
+      <c r="J7">
+        <v>500</v>
+      </c>
+      <c r="K7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>1863.34</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8">
+        <v>1863.34</v>
+      </c>
+      <c r="I8">
+        <v>50</v>
+      </c>
+      <c r="J8">
+        <v>500</v>
+      </c>
+      <c r="K8">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>25</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>1863.34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9">
+        <v>1863.34</v>
+      </c>
+      <c r="I9">
+        <v>50</v>
+      </c>
+      <c r="J9">
+        <v>500</v>
+      </c>
+      <c r="K9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>1863.34</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10">
+        <v>1863.34</v>
+      </c>
+      <c r="I10">
+        <v>50</v>
+      </c>
+      <c r="J10">
+        <v>500</v>
+      </c>
+      <c r="K10">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>1863.34</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11">
+        <v>1863.34</v>
+      </c>
+      <c r="I11">
+        <v>50</v>
+      </c>
+      <c r="J11">
+        <v>500</v>
+      </c>
+      <c r="K11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>1863.34</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12">
+        <v>1863.34</v>
+      </c>
+      <c r="I12">
+        <v>50</v>
+      </c>
+      <c r="J12">
+        <v>500</v>
+      </c>
+      <c r="K12">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>25</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>1863.34</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13">
+        <v>1863.34</v>
+      </c>
+      <c r="I13">
+        <v>50</v>
+      </c>
+      <c r="J13">
+        <v>500</v>
+      </c>
+      <c r="K13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>25</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>1863.34</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14">
+        <v>1863.34</v>
+      </c>
+      <c r="I14">
+        <v>50</v>
+      </c>
+      <c r="J14">
+        <v>500</v>
+      </c>
+      <c r="K14">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>25</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>1863.34</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15">
+        <v>1863.34</v>
+      </c>
+      <c r="I15">
+        <v>50</v>
+      </c>
+      <c r="J15">
+        <v>500</v>
+      </c>
+      <c r="K15">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>1863.34</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16">
+        <v>1863.34</v>
+      </c>
+      <c r="I16">
+        <v>50</v>
+      </c>
+      <c r="J16">
+        <v>500</v>
+      </c>
+      <c r="K16">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>25</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>1863.34</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17">
+        <v>1863.34</v>
+      </c>
+      <c r="I17">
+        <v>50</v>
+      </c>
+      <c r="J17">
+        <v>500</v>
+      </c>
+      <c r="K17">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>25</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>1863.34</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18">
+        <v>1863.34</v>
+      </c>
+      <c r="I18">
+        <v>50</v>
+      </c>
+      <c r="J18">
+        <v>500</v>
+      </c>
+      <c r="K18">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>25</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>1863.34</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19">
+        <v>1863.34</v>
+      </c>
+      <c r="I19">
+        <v>50</v>
+      </c>
+      <c r="J19">
+        <v>500</v>
+      </c>
+      <c r="K19">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>25</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>1863.34</v>
+      </c>
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20">
+        <v>1863.34</v>
+      </c>
+      <c r="I20">
+        <v>50</v>
+      </c>
+      <c r="J20">
+        <v>500</v>
+      </c>
+      <c r="K20">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>25</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>1863.34</v>
+      </c>
+      <c r="G21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21">
+        <v>1863.34</v>
+      </c>
+      <c r="I21">
+        <v>50</v>
+      </c>
+      <c r="J21">
+        <v>500</v>
+      </c>
+      <c r="K21">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22">
+        <v>1863.34</v>
+      </c>
+      <c r="G22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22">
+        <v>1863.34</v>
+      </c>
+      <c r="I22">
+        <v>50</v>
+      </c>
+      <c r="J22">
+        <v>500</v>
+      </c>
+      <c r="K22">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>25</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23">
+        <v>1863.34</v>
+      </c>
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23">
+        <v>1863.34</v>
+      </c>
+      <c r="I23">
+        <v>50</v>
+      </c>
+      <c r="J23">
+        <v>500</v>
+      </c>
+      <c r="K23">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>25</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>1863.34</v>
+      </c>
+      <c r="G24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24">
+        <v>1863.34</v>
+      </c>
+      <c r="I24">
+        <v>50</v>
+      </c>
+      <c r="J24">
+        <v>500</v>
+      </c>
+      <c r="K24">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>27</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>25</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>1863.34</v>
+      </c>
+      <c r="G25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25">
+        <v>1863.34</v>
+      </c>
+      <c r="I25">
+        <v>50</v>
+      </c>
+      <c r="J25">
+        <v>500</v>
+      </c>
+      <c r="K25">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>28</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>1863.34</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26">
+        <v>1863.34</v>
+      </c>
+      <c r="I26">
+        <v>50</v>
+      </c>
+      <c r="J26">
+        <v>500</v>
+      </c>
+      <c r="K26">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>29</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>25</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>1863.34</v>
+      </c>
+      <c r="G27" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27">
+        <v>1863.34</v>
+      </c>
+      <c r="I27">
+        <v>50</v>
+      </c>
+      <c r="J27">
+        <v>500</v>
+      </c>
+      <c r="K27">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>30</v>
+      </c>
+      <c r="C28">
+        <v>10</v>
+      </c>
+      <c r="D28">
+        <v>25</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="F28">
+        <v>1863.34</v>
+      </c>
+      <c r="G28" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28">
+        <v>1863.34</v>
+      </c>
+      <c r="I28">
+        <v>50</v>
+      </c>
+      <c r="J28">
+        <v>500</v>
+      </c>
+      <c r="K28">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>31</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>25</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29">
+        <v>1863.34</v>
+      </c>
+      <c r="G29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29">
+        <v>1863.34</v>
+      </c>
+      <c r="I29">
+        <v>50</v>
+      </c>
+      <c r="J29">
+        <v>500</v>
+      </c>
+      <c r="K29">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>32</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>25</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="F30">
+        <v>1863.34</v>
+      </c>
+      <c r="G30" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30">
+        <v>1863.34</v>
+      </c>
+      <c r="I30">
+        <v>50</v>
+      </c>
+      <c r="J30">
+        <v>500</v>
+      </c>
+      <c r="K30">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>33</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>25</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>1863.34</v>
+      </c>
+      <c r="G31" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31">
+        <v>1863.34</v>
+      </c>
+      <c r="I31">
+        <v>50</v>
+      </c>
+      <c r="J31">
+        <v>500</v>
+      </c>
+      <c r="K31">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>34</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>25</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32">
+        <v>1863.34</v>
+      </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32">
+        <v>1863.34</v>
+      </c>
+      <c r="I32">
+        <v>50</v>
+      </c>
+      <c r="J32">
+        <v>500</v>
+      </c>
+      <c r="K32">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>35</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>25</v>
+      </c>
+      <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <v>1863.34</v>
+      </c>
+      <c r="G33" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33">
+        <v>1863.34</v>
+      </c>
+      <c r="I33">
+        <v>50</v>
+      </c>
+      <c r="J33">
+        <v>500</v>
+      </c>
+      <c r="K33">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>36</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>25</v>
+      </c>
+      <c r="E34">
+        <v>5</v>
+      </c>
+      <c r="F34">
+        <v>1863.34</v>
+      </c>
+      <c r="G34" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34">
+        <v>1863.34</v>
+      </c>
+      <c r="I34">
+        <v>50</v>
+      </c>
+      <c r="J34">
+        <v>500</v>
+      </c>
+      <c r="K34">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>37</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>25</v>
+      </c>
+      <c r="E35">
+        <v>5</v>
+      </c>
+      <c r="F35">
+        <v>1863.34</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35">
+        <v>1863.34</v>
+      </c>
+      <c r="I35">
+        <v>50</v>
+      </c>
+      <c r="J35">
+        <v>500</v>
+      </c>
+      <c r="K35">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>38</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="D36">
+        <v>25</v>
+      </c>
+      <c r="E36">
+        <v>5</v>
+      </c>
+      <c r="F36">
+        <v>1863.34</v>
+      </c>
+      <c r="G36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36">
+        <v>1863.34</v>
+      </c>
+      <c r="I36">
+        <v>50</v>
+      </c>
+      <c r="J36">
+        <v>500</v>
+      </c>
+      <c r="K36">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>39</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
+      </c>
+      <c r="D37">
+        <v>25</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
+      </c>
+      <c r="F37">
+        <v>1863.34</v>
+      </c>
+      <c r="G37" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37">
+        <v>1863.34</v>
+      </c>
+      <c r="I37">
+        <v>50</v>
+      </c>
+      <c r="J37">
+        <v>500</v>
+      </c>
+      <c r="K37">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>40</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38">
+        <v>25</v>
+      </c>
+      <c r="E38">
+        <v>5</v>
+      </c>
+      <c r="F38">
+        <v>1863.34</v>
+      </c>
+      <c r="G38" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38">
+        <v>1863.34</v>
+      </c>
+      <c r="I38">
+        <v>50</v>
+      </c>
+      <c r="J38">
+        <v>500</v>
+      </c>
+      <c r="K38">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>41</v>
+      </c>
+      <c r="C39">
+        <v>10</v>
+      </c>
+      <c r="D39">
+        <v>25</v>
+      </c>
+      <c r="E39">
+        <v>5</v>
+      </c>
+      <c r="F39">
+        <v>1863.34</v>
+      </c>
+      <c r="G39" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39">
+        <v>1863.34</v>
+      </c>
+      <c r="I39">
+        <v>50</v>
+      </c>
+      <c r="J39">
+        <v>500</v>
+      </c>
+      <c r="K39">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>42</v>
+      </c>
+      <c r="C40">
+        <v>10</v>
+      </c>
+      <c r="D40">
+        <v>25</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40">
+        <v>1863.34</v>
+      </c>
+      <c r="G40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40">
+        <v>1863.34</v>
+      </c>
+      <c r="I40">
+        <v>50</v>
+      </c>
+      <c r="J40">
+        <v>500</v>
+      </c>
+      <c r="K40">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>43</v>
+      </c>
+      <c r="C41">
+        <v>10</v>
+      </c>
+      <c r="D41">
+        <v>25</v>
+      </c>
+      <c r="E41">
+        <v>5</v>
+      </c>
+      <c r="F41">
+        <v>1863.34</v>
+      </c>
+      <c r="G41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41">
+        <v>1863.34</v>
+      </c>
+      <c r="I41">
+        <v>50</v>
+      </c>
+      <c r="J41">
+        <v>500</v>
+      </c>
+      <c r="K41">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>44</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+      <c r="D42">
+        <v>25</v>
+      </c>
+      <c r="E42">
+        <v>5</v>
+      </c>
+      <c r="F42">
+        <v>1863.34</v>
+      </c>
+      <c r="G42" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42">
+        <v>1863.34</v>
+      </c>
+      <c r="I42">
+        <v>50</v>
+      </c>
+      <c r="J42">
+        <v>500</v>
+      </c>
+      <c r="K42">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>45</v>
+      </c>
+      <c r="C43">
+        <v>10</v>
+      </c>
+      <c r="D43">
+        <v>25</v>
+      </c>
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="F43">
+        <v>1863.34</v>
+      </c>
+      <c r="G43" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43">
+        <v>1863.34</v>
+      </c>
+      <c r="I43">
+        <v>50</v>
+      </c>
+      <c r="J43">
+        <v>500</v>
+      </c>
+      <c r="K43">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>46</v>
+      </c>
+      <c r="C44">
+        <v>10</v>
+      </c>
+      <c r="D44">
+        <v>25</v>
+      </c>
+      <c r="E44">
+        <v>5</v>
+      </c>
+      <c r="F44">
+        <v>1863.34</v>
+      </c>
+      <c r="G44" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44">
+        <v>1863.34</v>
+      </c>
+      <c r="I44">
+        <v>50</v>
+      </c>
+      <c r="J44">
+        <v>500</v>
+      </c>
+      <c r="K44">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>47</v>
+      </c>
+      <c r="C45">
+        <v>10</v>
+      </c>
+      <c r="D45">
+        <v>25</v>
+      </c>
+      <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="F45">
+        <v>1863.34</v>
+      </c>
+      <c r="G45" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45">
+        <v>1863.34</v>
+      </c>
+      <c r="I45">
+        <v>50</v>
+      </c>
+      <c r="J45">
+        <v>500</v>
+      </c>
+      <c r="K45">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>5</v>
+      </c>
+      <c r="B46">
+        <v>48</v>
+      </c>
+      <c r="C46">
+        <v>10</v>
+      </c>
+      <c r="D46">
+        <v>25</v>
+      </c>
+      <c r="E46">
+        <v>5</v>
+      </c>
+      <c r="F46">
+        <v>1863.34</v>
+      </c>
+      <c r="G46" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46">
+        <v>1863.34</v>
+      </c>
+      <c r="I46">
+        <v>50</v>
+      </c>
+      <c r="J46">
+        <v>500</v>
+      </c>
+      <c r="K46">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>5</v>
+      </c>
+      <c r="B47">
+        <v>49</v>
+      </c>
+      <c r="C47">
+        <v>10</v>
+      </c>
+      <c r="D47">
+        <v>25</v>
+      </c>
+      <c r="E47">
+        <v>5</v>
+      </c>
+      <c r="F47">
+        <v>1863.34</v>
+      </c>
+      <c r="G47" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47">
+        <v>1863.34</v>
+      </c>
+      <c r="I47">
+        <v>50</v>
+      </c>
+      <c r="J47">
+        <v>500</v>
+      </c>
+      <c r="K47">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>50</v>
+      </c>
+      <c r="C48">
+        <v>10</v>
+      </c>
+      <c r="D48">
+        <v>25</v>
+      </c>
+      <c r="E48">
+        <v>5</v>
+      </c>
+      <c r="F48">
+        <v>1863.34</v>
+      </c>
+      <c r="G48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48">
+        <v>1863.34</v>
+      </c>
+      <c r="I48">
+        <v>50</v>
+      </c>
+      <c r="J48">
+        <v>500</v>
+      </c>
+      <c r="K48">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#14 #13 Excel and OnePath
</commit_message>
<xml_diff>
--- a/Batch_Szenarios.xlsx
+++ b/Batch_Szenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/55b5a83da9441d2b/Business/Ressourcen/GitRepos/M-K/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{35E7D29B-4C7C-4EB1-95F5-C9C6FB77E031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86C74CF4-1A42-4D7D-9415-6F74CFDB2246}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{35E7D29B-4C7C-4EB1-95F5-C9C6FB77E031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{050DFCE1-EE36-482D-9E70-6ABA10AB29D3}"/>
   <bookViews>
-    <workbookView xWindow="10215" yWindow="4500" windowWidth="37275" windowHeight="13515" xr2:uid="{84012C3F-0F01-4CE2-BC25-ED3D97AAB7AF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{84012C3F-0F01-4CE2-BC25-ED3D97AAB7AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Batch_Szenarios" sheetId="2" r:id="rId1"/>
@@ -485,26 +485,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B72C522-7B1A-48D2-B2EE-FC13DB351A8C}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -539,7 +539,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>5</v>
       </c>
@@ -571,15 +571,15 @@
         <v>500</v>
       </c>
       <c r="K2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -606,15 +606,15 @@
         <v>500</v>
       </c>
       <c r="K3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -641,15 +641,15 @@
         <v>500</v>
       </c>
       <c r="K4">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -676,15 +676,15 @@
         <v>500</v>
       </c>
       <c r="K5">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -711,15 +711,15 @@
         <v>500</v>
       </c>
       <c r="K6">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -746,15 +746,15 @@
         <v>500</v>
       </c>
       <c r="K7">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -781,15 +781,15 @@
         <v>500</v>
       </c>
       <c r="K8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -816,15 +816,15 @@
         <v>500</v>
       </c>
       <c r="K9">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>5</v>
       </c>
       <c r="B10">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -851,15 +851,15 @@
         <v>500</v>
       </c>
       <c r="K10">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>5</v>
       </c>
       <c r="B11">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -886,15 +886,15 @@
         <v>500</v>
       </c>
       <c r="K11">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>5</v>
       </c>
       <c r="B12">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -921,15 +921,15 @@
         <v>500</v>
       </c>
       <c r="K12">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>5</v>
       </c>
       <c r="B13">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -956,15 +956,15 @@
         <v>500</v>
       </c>
       <c r="K13">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>5</v>
       </c>
       <c r="B14">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <v>10</v>
@@ -991,15 +991,15 @@
         <v>500</v>
       </c>
       <c r="K14">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>5</v>
       </c>
       <c r="B15">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C15">
         <v>10</v>
@@ -1026,15 +1026,15 @@
         <v>500</v>
       </c>
       <c r="K15">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>5</v>
       </c>
       <c r="B16">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -1061,15 +1061,15 @@
         <v>500</v>
       </c>
       <c r="K16">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>5</v>
       </c>
       <c r="B17">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>10</v>
@@ -1096,15 +1096,15 @@
         <v>500</v>
       </c>
       <c r="K17">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>5</v>
       </c>
       <c r="B18">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C18">
         <v>10</v>
@@ -1131,15 +1131,15 @@
         <v>500</v>
       </c>
       <c r="K18">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>5</v>
       </c>
       <c r="B19">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C19">
         <v>10</v>
@@ -1166,15 +1166,15 @@
         <v>500</v>
       </c>
       <c r="K19">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>5</v>
       </c>
       <c r="B20">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C20">
         <v>10</v>
@@ -1201,15 +1201,15 @@
         <v>500</v>
       </c>
       <c r="K20">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>5</v>
       </c>
       <c r="B21">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C21">
         <v>10</v>
@@ -1236,15 +1236,15 @@
         <v>500</v>
       </c>
       <c r="K21">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>5</v>
       </c>
       <c r="B22">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C22">
         <v>10</v>
@@ -1271,15 +1271,15 @@
         <v>500</v>
       </c>
       <c r="K22">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>5</v>
       </c>
       <c r="B23">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C23">
         <v>10</v>
@@ -1306,15 +1306,15 @@
         <v>500</v>
       </c>
       <c r="K23">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>5</v>
       </c>
       <c r="B24">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C24">
         <v>10</v>
@@ -1341,15 +1341,15 @@
         <v>500</v>
       </c>
       <c r="K24">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>5</v>
       </c>
       <c r="B25">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C25">
         <v>10</v>
@@ -1376,15 +1376,15 @@
         <v>500</v>
       </c>
       <c r="K25">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>5</v>
       </c>
       <c r="B26">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C26">
         <v>10</v>
@@ -1411,15 +1411,15 @@
         <v>500</v>
       </c>
       <c r="K26">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>5</v>
       </c>
       <c r="B27">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="C27">
         <v>10</v>
@@ -1446,15 +1446,15 @@
         <v>500</v>
       </c>
       <c r="K27">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>5</v>
       </c>
       <c r="B28">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C28">
         <v>10</v>
@@ -1481,15 +1481,15 @@
         <v>500</v>
       </c>
       <c r="K28">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>5</v>
       </c>
       <c r="B29">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="C29">
         <v>10</v>
@@ -1516,15 +1516,15 @@
         <v>500</v>
       </c>
       <c r="K29">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>5</v>
       </c>
       <c r="B30">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="C30">
         <v>10</v>
@@ -1551,15 +1551,15 @@
         <v>500</v>
       </c>
       <c r="K30">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>5</v>
       </c>
       <c r="B31">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="C31">
         <v>10</v>
@@ -1586,15 +1586,15 @@
         <v>500</v>
       </c>
       <c r="K31">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>5</v>
       </c>
       <c r="B32">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="C32">
         <v>10</v>
@@ -1621,15 +1621,15 @@
         <v>500</v>
       </c>
       <c r="K32">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>5</v>
       </c>
       <c r="B33">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C33">
         <v>10</v>
@@ -1656,15 +1656,15 @@
         <v>500</v>
       </c>
       <c r="K33">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>5</v>
       </c>
       <c r="B34">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="C34">
         <v>10</v>
@@ -1691,15 +1691,15 @@
         <v>500</v>
       </c>
       <c r="K34">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>5</v>
       </c>
       <c r="B35">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C35">
         <v>10</v>
@@ -1726,15 +1726,15 @@
         <v>500</v>
       </c>
       <c r="K35">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>5</v>
       </c>
       <c r="B36">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="C36">
         <v>10</v>
@@ -1761,15 +1761,15 @@
         <v>500</v>
       </c>
       <c r="K36">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>5</v>
       </c>
       <c r="B37">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="C37">
         <v>10</v>
@@ -1796,15 +1796,15 @@
         <v>500</v>
       </c>
       <c r="K37">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>5</v>
       </c>
       <c r="B38">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="C38">
         <v>10</v>
@@ -1831,15 +1831,15 @@
         <v>500</v>
       </c>
       <c r="K38">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>5</v>
       </c>
       <c r="B39">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="C39">
         <v>10</v>
@@ -1866,15 +1866,15 @@
         <v>500</v>
       </c>
       <c r="K39">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>5</v>
       </c>
       <c r="B40">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="C40">
         <v>10</v>
@@ -1901,15 +1901,15 @@
         <v>500</v>
       </c>
       <c r="K40">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>5</v>
       </c>
       <c r="B41">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="C41">
         <v>10</v>
@@ -1936,15 +1936,15 @@
         <v>500</v>
       </c>
       <c r="K41">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>5</v>
       </c>
       <c r="B42">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="C42">
         <v>10</v>
@@ -1971,15 +1971,15 @@
         <v>500</v>
       </c>
       <c r="K42">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>5</v>
       </c>
       <c r="B43">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C43">
         <v>10</v>
@@ -2006,15 +2006,15 @@
         <v>500</v>
       </c>
       <c r="K43">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>5</v>
       </c>
       <c r="B44">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="C44">
         <v>10</v>
@@ -2041,15 +2041,15 @@
         <v>500</v>
       </c>
       <c r="K44">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>5</v>
       </c>
       <c r="B45">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="C45">
         <v>10</v>
@@ -2076,15 +2076,15 @@
         <v>500</v>
       </c>
       <c r="K45">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>5</v>
       </c>
       <c r="B46">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="C46">
         <v>10</v>
@@ -2111,15 +2111,15 @@
         <v>500</v>
       </c>
       <c r="K46">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>5</v>
       </c>
       <c r="B47">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C47">
         <v>10</v>
@@ -2146,15 +2146,15 @@
         <v>500</v>
       </c>
       <c r="K47">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>5</v>
       </c>
       <c r="B48">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="C48">
         <v>10</v>
@@ -2181,7 +2181,7 @@
         <v>500</v>
       </c>
       <c r="K48">
-        <v>2000</v>
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
@@ -2200,7 +2200,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>